<commit_message>
Final additions to scales
</commit_message>
<xml_diff>
--- a/software/o_c_REV/resources/Xen-harmonic.xlsx
+++ b/software/o_c_REV/resources/Xen-harmonic.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="105">
   <si>
     <t>Step</t>
   </si>
@@ -259,6 +259,90 @@
   <si>
     <t>13 TET Father[8]</t>
   </si>
+  <si>
+    <t>15 TET Blackwood[10]</t>
+  </si>
+  <si>
+    <t>16 TET Mavila[7]</t>
+  </si>
+  <si>
+    <t>16 TET Mavila[9]</t>
+  </si>
+  <si>
+    <t>17 TET Superpyth[12]</t>
+  </si>
+  <si>
+    <t>22 TET Orwell[9]</t>
+  </si>
+  <si>
+    <t>22 TET Pajara[10] Static Symmetrical Maj</t>
+  </si>
+  <si>
+    <t>22 TET Pajara[10] Std Pentachordal Maj</t>
+  </si>
+  <si>
+    <t>22 TET Porcupine[7]</t>
+  </si>
+  <si>
+    <t>26 TET Flattone[12]</t>
+  </si>
+  <si>
+    <t>26 TET Lemba[10]</t>
+  </si>
+  <si>
+    <t>46 TET Sensi[11]</t>
+  </si>
+  <si>
+    <t>53 TET Orwell[9]</t>
+  </si>
+  <si>
+    <t>12 out of 72-TET scale by Prent Rodgers</t>
+  </si>
+  <si>
+    <t>Trivalent scale in zeus temperament; thirds are all {7/6, 6/5, 5/4}; 99et tuning;</t>
+  </si>
+  <si>
+    <t>313 TET elfmadagasgar[9]</t>
+  </si>
+  <si>
+    <t>Marvel woo version of glumma</t>
+  </si>
+  <si>
+    <t>TOP Parapyth[12]</t>
+  </si>
+  <si>
+    <t>Hirajoshi[5]</t>
+  </si>
+  <si>
+    <t>Scottish bagpipes</t>
+  </si>
+  <si>
+    <t>Thai ranat</t>
+  </si>
+  <si>
+    <t>Tartini-Vallotti</t>
+  </si>
+  <si>
+    <t>13 out of 22-tET, generator = 5</t>
+  </si>
+  <si>
+    <t>13 out of 19-tET, Mandelbaum</t>
+  </si>
+  <si>
+    <t>Magic[16] in 145-tET</t>
+  </si>
+  <si>
+    <t>g=9 steps of 139-tET. Gene Ward Smith "Quartaminorthirds" 7-limit temperament</t>
+  </si>
+  <si>
+    <t>Armodue semi-equalizzato</t>
+  </si>
+  <si>
+    <t>Huygens</t>
+  </si>
+  <si>
+    <t>202 TET tempering of octone</t>
+  </si>
 </sst>
 </file>
 
@@ -318,8 +402,78 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -458,7 +612,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -524,6 +678,41 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -589,6 +778,41 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -864,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y434"/>
+  <dimension ref="A1:Y669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="C436" sqref="C436"/>
+    <sheetView tabSelected="1" topLeftCell="A557" workbookViewId="0">
+      <selection activeCell="A580" sqref="A580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11475,7 +11699,7 @@
         <v>1181.5384576000001</v>
       </c>
     </row>
-    <row r="433" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="433" spans="3:14" x14ac:dyDescent="0.2">
       <c r="G433" s="3">
         <v>7</v>
       </c>
@@ -11487,7 +11711,7 @@
         <v>1417.8461567999998</v>
       </c>
     </row>
-    <row r="434" spans="7:9" x14ac:dyDescent="0.2">
+    <row r="434" spans="3:14" x14ac:dyDescent="0.2">
       <c r="G434" s="3">
         <v>8</v>
       </c>
@@ -11496,6 +11720,4007 @@
       </c>
       <c r="I434" s="1">
         <f t="shared" si="70"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="435" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C435" s="1"/>
+      <c r="D435" s="1"/>
+      <c r="E435" s="1"/>
+      <c r="F435" s="1"/>
+      <c r="G435" s="1"/>
+      <c r="H435" s="1"/>
+      <c r="I435" s="1"/>
+      <c r="J435" s="1"/>
+      <c r="K435" s="1"/>
+      <c r="L435" s="1"/>
+      <c r="M435" s="1"/>
+      <c r="N435" s="1"/>
+    </row>
+    <row r="436" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C436" t="s">
+        <v>77</v>
+      </c>
+      <c r="G436" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H436" s="3"/>
+      <c r="I436" s="1"/>
+    </row>
+    <row r="437" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C437" s="3"/>
+      <c r="D437" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E437" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G437" s="3"/>
+      <c r="H437" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I437" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="438" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C438" s="3">
+        <v>0</v>
+      </c>
+      <c r="D438" s="3">
+        <v>0</v>
+      </c>
+      <c r="E438" s="1">
+        <f>(D438/$D$448)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G438" s="3">
+        <v>0</v>
+      </c>
+      <c r="H438" s="3">
+        <v>0</v>
+      </c>
+      <c r="I438" s="1">
+        <f>(H438/$H$445)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C439" s="3">
+        <v>1</v>
+      </c>
+      <c r="D439" s="3">
+        <v>160</v>
+      </c>
+      <c r="E439" s="1">
+        <f t="shared" ref="E439:E448" si="71">(D439/$D$448)*1536</f>
+        <v>204.8</v>
+      </c>
+      <c r="G439" s="3">
+        <v>1</v>
+      </c>
+      <c r="H439" s="3">
+        <v>150</v>
+      </c>
+      <c r="I439" s="1">
+        <f t="shared" ref="I439:I445" si="72">(H439/$H$445)*1536</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="440" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C440" s="3">
+        <v>2</v>
+      </c>
+      <c r="D440" s="3">
+        <v>240</v>
+      </c>
+      <c r="E440" s="1">
+        <f t="shared" si="71"/>
+        <v>307.20000000000005</v>
+      </c>
+      <c r="G440" s="3">
+        <v>2</v>
+      </c>
+      <c r="H440" s="3">
+        <v>300</v>
+      </c>
+      <c r="I440" s="1">
+        <f t="shared" si="72"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="441" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C441" s="3">
+        <v>3</v>
+      </c>
+      <c r="D441" s="3">
+        <v>400</v>
+      </c>
+      <c r="E441" s="1">
+        <f t="shared" si="71"/>
+        <v>512</v>
+      </c>
+      <c r="G441" s="3">
+        <v>3</v>
+      </c>
+      <c r="H441" s="3">
+        <v>525</v>
+      </c>
+      <c r="I441" s="1">
+        <f t="shared" si="72"/>
+        <v>672</v>
+      </c>
+    </row>
+    <row r="442" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C442" s="3">
+        <v>4</v>
+      </c>
+      <c r="D442" s="3">
+        <v>480</v>
+      </c>
+      <c r="E442" s="1">
+        <f t="shared" si="71"/>
+        <v>614.40000000000009</v>
+      </c>
+      <c r="G442" s="3">
+        <v>4</v>
+      </c>
+      <c r="H442" s="3">
+        <v>675</v>
+      </c>
+      <c r="I442" s="1">
+        <f t="shared" si="72"/>
+        <v>864</v>
+      </c>
+    </row>
+    <row r="443" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C443" s="3">
+        <v>5</v>
+      </c>
+      <c r="D443" s="3">
+        <v>640</v>
+      </c>
+      <c r="E443" s="1">
+        <f t="shared" si="71"/>
+        <v>819.2</v>
+      </c>
+      <c r="G443" s="3">
+        <v>5</v>
+      </c>
+      <c r="H443" s="3">
+        <v>825</v>
+      </c>
+      <c r="I443" s="1">
+        <f t="shared" si="72"/>
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="444" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C444" s="3">
+        <v>6</v>
+      </c>
+      <c r="D444" s="3">
+        <v>720</v>
+      </c>
+      <c r="E444" s="1">
+        <f t="shared" si="71"/>
+        <v>921.59999999999991</v>
+      </c>
+      <c r="G444" s="3">
+        <v>6</v>
+      </c>
+      <c r="H444" s="3">
+        <v>975</v>
+      </c>
+      <c r="I444" s="1">
+        <f t="shared" si="72"/>
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="445" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C445" s="3">
+        <v>7</v>
+      </c>
+      <c r="D445" s="3">
+        <v>880</v>
+      </c>
+      <c r="E445" s="1">
+        <f t="shared" si="71"/>
+        <v>1126.3999999999999</v>
+      </c>
+      <c r="G445" s="3">
+        <v>7</v>
+      </c>
+      <c r="H445" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I445" s="1">
+        <f t="shared" si="72"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="446" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C446" s="3">
+        <v>8</v>
+      </c>
+      <c r="D446" s="3">
+        <v>960</v>
+      </c>
+      <c r="E446" s="1">
+        <f t="shared" si="71"/>
+        <v>1228.8000000000002</v>
+      </c>
+      <c r="G446" s="3"/>
+      <c r="H446" s="3"/>
+      <c r="I446" s="1"/>
+    </row>
+    <row r="447" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C447" s="3">
+        <v>9</v>
+      </c>
+      <c r="D447">
+        <v>1120</v>
+      </c>
+      <c r="E447" s="1">
+        <f t="shared" si="71"/>
+        <v>1433.6</v>
+      </c>
+      <c r="G447" s="1"/>
+      <c r="H447" s="1"/>
+      <c r="I447" s="1"/>
+      <c r="J447" s="1"/>
+      <c r="K447" s="1"/>
+      <c r="L447" s="1"/>
+      <c r="M447" s="1"/>
+    </row>
+    <row r="448" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C448" s="3">
+        <v>10</v>
+      </c>
+      <c r="D448" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E448" s="1">
+        <f t="shared" si="71"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="449" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C449" s="1"/>
+      <c r="D449" s="1"/>
+      <c r="E449" s="1"/>
+      <c r="F449" s="1"/>
+      <c r="G449" s="1"/>
+      <c r="H449" s="1"/>
+      <c r="I449" s="1"/>
+      <c r="J449" s="1"/>
+      <c r="K449" s="1"/>
+      <c r="L449" s="1"/>
+    </row>
+    <row r="451" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C451" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D451" s="3"/>
+      <c r="E451" s="1"/>
+      <c r="G451" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="452" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C452" s="3"/>
+      <c r="D452" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E452" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G452" s="3"/>
+      <c r="H452" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I452" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="453" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C453" s="3">
+        <v>0</v>
+      </c>
+      <c r="D453" s="3">
+        <v>0</v>
+      </c>
+      <c r="E453" s="1">
+        <f>(D453/$D$462)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G453" s="3">
+        <v>0</v>
+      </c>
+      <c r="H453" s="3">
+        <v>0</v>
+      </c>
+      <c r="I453" s="1">
+        <f>(H453/$H$465)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C454" s="3">
+        <v>1</v>
+      </c>
+      <c r="D454" s="3">
+        <v>75</v>
+      </c>
+      <c r="E454" s="1">
+        <f t="shared" ref="E454:E462" si="73">(D454/$D$462)*1536</f>
+        <v>96</v>
+      </c>
+      <c r="G454" s="3">
+        <v>1</v>
+      </c>
+      <c r="H454" s="3">
+        <v>70.588239999999999</v>
+      </c>
+      <c r="I454" s="1">
+        <f t="shared" ref="I454:I465" si="74">(H454/$H$465)*1536</f>
+        <v>90.352947199999988</v>
+      </c>
+    </row>
+    <row r="455" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C455" s="3">
+        <v>2</v>
+      </c>
+      <c r="D455" s="3">
+        <v>225</v>
+      </c>
+      <c r="E455" s="1">
+        <f t="shared" si="73"/>
+        <v>288</v>
+      </c>
+      <c r="G455" s="3">
+        <v>2</v>
+      </c>
+      <c r="H455" s="3">
+        <v>141.17646999999999</v>
+      </c>
+      <c r="I455" s="1">
+        <f t="shared" si="74"/>
+        <v>180.7058816</v>
+      </c>
+    </row>
+    <row r="456" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C456" s="3">
+        <v>3</v>
+      </c>
+      <c r="D456" s="3">
+        <v>375</v>
+      </c>
+      <c r="E456" s="1">
+        <f t="shared" si="73"/>
+        <v>480</v>
+      </c>
+      <c r="G456" s="3">
+        <v>3</v>
+      </c>
+      <c r="H456" s="3">
+        <v>282.35293999999999</v>
+      </c>
+      <c r="I456" s="1">
+        <f t="shared" si="74"/>
+        <v>361.4117632</v>
+      </c>
+    </row>
+    <row r="457" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C457" s="3">
+        <v>4</v>
+      </c>
+      <c r="D457" s="3">
+        <v>525</v>
+      </c>
+      <c r="E457" s="1">
+        <f t="shared" si="73"/>
+        <v>672</v>
+      </c>
+      <c r="G457" s="3">
+        <v>4</v>
+      </c>
+      <c r="H457" s="3">
+        <v>352.94117999999997</v>
+      </c>
+      <c r="I457" s="1">
+        <f t="shared" si="74"/>
+        <v>451.7647103999999</v>
+      </c>
+    </row>
+    <row r="458" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C458" s="3">
+        <v>5</v>
+      </c>
+      <c r="D458" s="3">
+        <v>600</v>
+      </c>
+      <c r="E458" s="1">
+        <f t="shared" si="73"/>
+        <v>768</v>
+      </c>
+      <c r="G458" s="3">
+        <v>5</v>
+      </c>
+      <c r="H458" s="3">
+        <v>494.11765000000003</v>
+      </c>
+      <c r="I458" s="1">
+        <f t="shared" si="74"/>
+        <v>632.47059200000001</v>
+      </c>
+    </row>
+    <row r="459" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C459" s="3">
+        <v>6</v>
+      </c>
+      <c r="D459" s="3">
+        <v>750</v>
+      </c>
+      <c r="E459" s="1">
+        <f t="shared" si="73"/>
+        <v>960</v>
+      </c>
+      <c r="G459" s="3">
+        <v>6</v>
+      </c>
+      <c r="H459" s="3">
+        <v>564.70587999999998</v>
+      </c>
+      <c r="I459" s="1">
+        <f t="shared" si="74"/>
+        <v>722.82352639999999</v>
+      </c>
+    </row>
+    <row r="460" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C460" s="3">
+        <v>7</v>
+      </c>
+      <c r="D460" s="3">
+        <v>900</v>
+      </c>
+      <c r="E460" s="1">
+        <f t="shared" si="73"/>
+        <v>1152</v>
+      </c>
+      <c r="G460" s="3">
+        <v>7</v>
+      </c>
+      <c r="H460" s="3">
+        <v>635.29412000000002</v>
+      </c>
+      <c r="I460" s="1">
+        <f t="shared" si="74"/>
+        <v>813.17647360000001</v>
+      </c>
+    </row>
+    <row r="461" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C461" s="3">
+        <v>8</v>
+      </c>
+      <c r="D461">
+        <v>1050</v>
+      </c>
+      <c r="E461" s="1">
+        <f t="shared" si="73"/>
+        <v>1344</v>
+      </c>
+      <c r="G461" s="3">
+        <v>8</v>
+      </c>
+      <c r="H461" s="3">
+        <v>776.47059000000002</v>
+      </c>
+      <c r="I461" s="1">
+        <f t="shared" si="74"/>
+        <v>993.88235520000001</v>
+      </c>
+    </row>
+    <row r="462" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C462" s="3">
+        <v>9</v>
+      </c>
+      <c r="D462" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E462" s="1">
+        <f t="shared" si="73"/>
+        <v>1536</v>
+      </c>
+      <c r="G462" s="3">
+        <v>9</v>
+      </c>
+      <c r="H462">
+        <v>847.05881999999997</v>
+      </c>
+      <c r="I462" s="1">
+        <f t="shared" si="74"/>
+        <v>1084.2352896</v>
+      </c>
+    </row>
+    <row r="463" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="G463" s="3">
+        <v>10</v>
+      </c>
+      <c r="H463" s="3">
+        <v>988.23528999999996</v>
+      </c>
+      <c r="I463" s="1">
+        <f t="shared" si="74"/>
+        <v>1264.9411712000001</v>
+      </c>
+    </row>
+    <row r="464" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="G464" s="3">
+        <v>11</v>
+      </c>
+      <c r="H464">
+        <v>1058.8235299999999</v>
+      </c>
+      <c r="I464" s="1">
+        <f t="shared" si="74"/>
+        <v>1355.2941183999999</v>
+      </c>
+    </row>
+    <row r="465" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="G465" s="3">
+        <v>12</v>
+      </c>
+      <c r="H465" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I465" s="1">
+        <f t="shared" si="74"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="466" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C466" s="1"/>
+      <c r="D466" s="1"/>
+      <c r="E466" s="1"/>
+      <c r="F466" s="1"/>
+      <c r="G466" s="1"/>
+      <c r="H466" s="1"/>
+      <c r="I466" s="1"/>
+      <c r="J466" s="1"/>
+      <c r="K466" s="1"/>
+    </row>
+    <row r="467" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="G467" s="1"/>
+      <c r="H467" s="1"/>
+      <c r="I467" s="1"/>
+      <c r="J467" s="1"/>
+      <c r="K467" s="1"/>
+      <c r="L467" s="1"/>
+      <c r="M467" s="1"/>
+      <c r="N467" s="1"/>
+      <c r="O467" s="1"/>
+      <c r="P467" s="1"/>
+      <c r="Q467" s="1"/>
+      <c r="R467" s="1"/>
+    </row>
+    <row r="469" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C469" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D469" s="3"/>
+      <c r="E469" s="1"/>
+      <c r="G469" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="470" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C470" s="3"/>
+      <c r="D470" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E470" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G470" s="3"/>
+      <c r="H470" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I470" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="471" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C471" s="3">
+        <v>0</v>
+      </c>
+      <c r="D471" s="3">
+        <v>0</v>
+      </c>
+      <c r="E471" s="1">
+        <f>(D471/$D$480)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G471" s="3">
+        <v>0</v>
+      </c>
+      <c r="H471" s="3">
+        <v>0</v>
+      </c>
+      <c r="I471" s="1">
+        <f>(H471/$H$481)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C472" s="3">
+        <v>1</v>
+      </c>
+      <c r="D472" s="3">
+        <v>109.09090999999999</v>
+      </c>
+      <c r="E472" s="1">
+        <f t="shared" ref="E472:E480" si="75">(D472/$D$480)*1536</f>
+        <v>139.6363648</v>
+      </c>
+      <c r="G472" s="3">
+        <v>1</v>
+      </c>
+      <c r="H472" s="3">
+        <v>109.09090999999999</v>
+      </c>
+      <c r="I472" s="1">
+        <f t="shared" ref="I472:I481" si="76">(H472/$H$481)*1536</f>
+        <v>139.6363648</v>
+      </c>
+    </row>
+    <row r="473" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C473" s="3">
+        <v>2</v>
+      </c>
+      <c r="D473" s="3">
+        <v>272.72726999999998</v>
+      </c>
+      <c r="E473" s="1">
+        <f t="shared" si="75"/>
+        <v>349.09090559999999</v>
+      </c>
+      <c r="G473" s="3">
+        <v>2</v>
+      </c>
+      <c r="H473" s="3">
+        <v>218.18181999999999</v>
+      </c>
+      <c r="I473" s="1">
+        <f t="shared" si="76"/>
+        <v>279.27272959999999</v>
+      </c>
+    </row>
+    <row r="474" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C474" s="3">
+        <v>3</v>
+      </c>
+      <c r="D474" s="3">
+        <v>381.81817999999998</v>
+      </c>
+      <c r="E474" s="1">
+        <f t="shared" si="75"/>
+        <v>488.72727040000001</v>
+      </c>
+      <c r="G474" s="3">
+        <v>3</v>
+      </c>
+      <c r="H474" s="3">
+        <v>381.81817999999998</v>
+      </c>
+      <c r="I474" s="1">
+        <f t="shared" si="76"/>
+        <v>488.72727040000001</v>
+      </c>
+    </row>
+    <row r="475" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C475" s="3">
+        <v>4</v>
+      </c>
+      <c r="D475" s="3">
+        <v>545.45455000000004</v>
+      </c>
+      <c r="E475" s="1">
+        <f t="shared" si="75"/>
+        <v>698.18182400000001</v>
+      </c>
+      <c r="G475" s="3">
+        <v>4</v>
+      </c>
+      <c r="H475" s="3">
+        <v>490.90908999999999</v>
+      </c>
+      <c r="I475" s="1">
+        <f t="shared" si="76"/>
+        <v>628.36363519999998</v>
+      </c>
+    </row>
+    <row r="476" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C476" s="3">
+        <v>5</v>
+      </c>
+      <c r="D476" s="3">
+        <v>654.54544999999996</v>
+      </c>
+      <c r="E476" s="1">
+        <f t="shared" si="75"/>
+        <v>837.81817599999999</v>
+      </c>
+      <c r="G476" s="3">
+        <v>5</v>
+      </c>
+      <c r="H476" s="3">
+        <v>600</v>
+      </c>
+      <c r="I476" s="1">
+        <f t="shared" si="76"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="477" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C477" s="3">
+        <v>6</v>
+      </c>
+      <c r="D477" s="3">
+        <v>818.18182000000002</v>
+      </c>
+      <c r="E477" s="1">
+        <f t="shared" si="75"/>
+        <v>1047.2727296</v>
+      </c>
+      <c r="G477" s="3">
+        <v>6</v>
+      </c>
+      <c r="H477" s="3">
+        <v>709.09091000000001</v>
+      </c>
+      <c r="I477" s="1">
+        <f t="shared" si="76"/>
+        <v>907.63636480000014</v>
+      </c>
+    </row>
+    <row r="478" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C478" s="3">
+        <v>7</v>
+      </c>
+      <c r="D478" s="3">
+        <v>927.27273000000002</v>
+      </c>
+      <c r="E478" s="1">
+        <f t="shared" si="75"/>
+        <v>1186.9090944</v>
+      </c>
+      <c r="G478" s="3">
+        <v>7</v>
+      </c>
+      <c r="H478" s="3">
+        <v>818.18182000000002</v>
+      </c>
+      <c r="I478" s="1">
+        <f t="shared" si="76"/>
+        <v>1047.2727296</v>
+      </c>
+    </row>
+    <row r="479" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C479" s="3">
+        <v>8</v>
+      </c>
+      <c r="D479">
+        <v>1090.9090900000001</v>
+      </c>
+      <c r="E479" s="1">
+        <f t="shared" si="75"/>
+        <v>1396.3636352000001</v>
+      </c>
+      <c r="G479" s="3">
+        <v>8</v>
+      </c>
+      <c r="H479" s="3">
+        <v>981.81817999999998</v>
+      </c>
+      <c r="I479" s="1">
+        <f t="shared" si="76"/>
+        <v>1256.7272704</v>
+      </c>
+    </row>
+    <row r="480" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C480" s="3">
+        <v>9</v>
+      </c>
+      <c r="D480" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E480" s="1">
+        <f t="shared" si="75"/>
+        <v>1536</v>
+      </c>
+      <c r="G480" s="3">
+        <v>9</v>
+      </c>
+      <c r="H480">
+        <v>1090.9090900000001</v>
+      </c>
+      <c r="I480" s="1">
+        <f t="shared" si="76"/>
+        <v>1396.3636352000001</v>
+      </c>
+    </row>
+    <row r="481" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="G481" s="3">
+        <v>10</v>
+      </c>
+      <c r="H481" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I481" s="1">
+        <f t="shared" si="76"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="482" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C482" s="1"/>
+      <c r="D482" s="1"/>
+      <c r="E482" s="1"/>
+      <c r="F482" s="1"/>
+      <c r="G482" s="4"/>
+      <c r="H482" s="1"/>
+      <c r="I482" s="1"/>
+      <c r="J482" s="1"/>
+      <c r="K482" s="1"/>
+      <c r="L482" s="1"/>
+    </row>
+    <row r="483" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="G483" s="3"/>
+      <c r="H483" s="3"/>
+      <c r="I483" s="1"/>
+    </row>
+    <row r="484" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C484" t="s">
+        <v>83</v>
+      </c>
+      <c r="G484" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H484" s="3"/>
+      <c r="I484" s="1"/>
+    </row>
+    <row r="485" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C485" s="3"/>
+      <c r="D485" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E485" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G485" s="3"/>
+      <c r="H485" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I485" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="486" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C486" s="3">
+        <v>0</v>
+      </c>
+      <c r="D486" s="3">
+        <v>0</v>
+      </c>
+      <c r="E486" s="1">
+        <f>(D486/$D$496)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G486" s="3">
+        <v>0</v>
+      </c>
+      <c r="H486" s="3">
+        <v>0</v>
+      </c>
+      <c r="I486" s="1">
+        <f>(H486/$H$493)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C487" s="3">
+        <v>1</v>
+      </c>
+      <c r="D487" s="3">
+        <v>109.09090999999999</v>
+      </c>
+      <c r="E487" s="1">
+        <f t="shared" ref="E487:E496" si="77">(D487/$D$496)*1536</f>
+        <v>139.6363648</v>
+      </c>
+      <c r="G487" s="3">
+        <v>1</v>
+      </c>
+      <c r="H487" s="3">
+        <v>163.63636</v>
+      </c>
+      <c r="I487" s="1">
+        <f t="shared" ref="I487:I493" si="78">(H487/$H$493)*1536</f>
+        <v>209.45454079999996</v>
+      </c>
+    </row>
+    <row r="488" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C488" s="3">
+        <v>2</v>
+      </c>
+      <c r="D488" s="3">
+        <v>218.18181999999999</v>
+      </c>
+      <c r="E488" s="1">
+        <f t="shared" si="77"/>
+        <v>279.27272959999999</v>
+      </c>
+      <c r="G488" s="3">
+        <v>2</v>
+      </c>
+      <c r="H488" s="3">
+        <v>327.27273000000002</v>
+      </c>
+      <c r="I488" s="1">
+        <f t="shared" si="78"/>
+        <v>418.90909440000007</v>
+      </c>
+    </row>
+    <row r="489" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C489" s="3">
+        <v>3</v>
+      </c>
+      <c r="D489" s="3">
+        <v>381.81817999999998</v>
+      </c>
+      <c r="E489" s="1">
+        <f t="shared" si="77"/>
+        <v>488.72727040000001</v>
+      </c>
+      <c r="G489" s="3">
+        <v>3</v>
+      </c>
+      <c r="H489" s="3">
+        <v>490.90908999999999</v>
+      </c>
+      <c r="I489" s="1">
+        <f t="shared" si="78"/>
+        <v>628.36363519999998</v>
+      </c>
+    </row>
+    <row r="490" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C490" s="3">
+        <v>4</v>
+      </c>
+      <c r="D490" s="3">
+        <v>490.90908999999999</v>
+      </c>
+      <c r="E490" s="1">
+        <f t="shared" si="77"/>
+        <v>628.36363519999998</v>
+      </c>
+      <c r="G490" s="3">
+        <v>4</v>
+      </c>
+      <c r="H490" s="3">
+        <v>709.09091000000001</v>
+      </c>
+      <c r="I490" s="1">
+        <f t="shared" si="78"/>
+        <v>907.63636480000014</v>
+      </c>
+    </row>
+    <row r="491" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C491" s="3">
+        <v>5</v>
+      </c>
+      <c r="D491" s="3">
+        <v>600</v>
+      </c>
+      <c r="E491" s="1">
+        <f t="shared" si="77"/>
+        <v>768</v>
+      </c>
+      <c r="G491" s="3">
+        <v>5</v>
+      </c>
+      <c r="H491" s="3">
+        <v>872.72726999999998</v>
+      </c>
+      <c r="I491" s="1">
+        <f t="shared" si="78"/>
+        <v>1117.0909056</v>
+      </c>
+    </row>
+    <row r="492" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C492" s="3">
+        <v>6</v>
+      </c>
+      <c r="D492" s="3">
+        <v>709.09091000000001</v>
+      </c>
+      <c r="E492" s="1">
+        <f t="shared" si="77"/>
+        <v>907.63636480000014</v>
+      </c>
+      <c r="G492" s="3">
+        <v>6</v>
+      </c>
+      <c r="H492" s="3">
+        <v>1036.36364</v>
+      </c>
+      <c r="I492" s="1">
+        <f t="shared" si="78"/>
+        <v>1326.5454592000001</v>
+      </c>
+    </row>
+    <row r="493" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C493" s="3">
+        <v>7</v>
+      </c>
+      <c r="D493" s="3">
+        <v>872.72726999999998</v>
+      </c>
+      <c r="E493" s="1">
+        <f t="shared" si="77"/>
+        <v>1117.0909056</v>
+      </c>
+      <c r="G493" s="3">
+        <v>7</v>
+      </c>
+      <c r="H493" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I493" s="1">
+        <f t="shared" si="78"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="494" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C494" s="3">
+        <v>8</v>
+      </c>
+      <c r="D494" s="3">
+        <v>981.81817999999998</v>
+      </c>
+      <c r="E494" s="1">
+        <f t="shared" si="77"/>
+        <v>1256.7272704</v>
+      </c>
+    </row>
+    <row r="495" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C495" s="3">
+        <v>9</v>
+      </c>
+      <c r="D495">
+        <v>1090.9090900000001</v>
+      </c>
+      <c r="E495" s="1">
+        <f t="shared" si="77"/>
+        <v>1396.3636352000001</v>
+      </c>
+      <c r="G495" s="1"/>
+      <c r="H495" s="1"/>
+      <c r="I495" s="1"/>
+      <c r="J495" s="1"/>
+      <c r="K495" s="1"/>
+      <c r="L495" s="1"/>
+      <c r="M495" s="1"/>
+    </row>
+    <row r="496" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C496" s="3">
+        <v>10</v>
+      </c>
+      <c r="D496" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E496" s="1">
+        <f t="shared" si="77"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="498" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C498" s="1"/>
+      <c r="D498" s="1"/>
+      <c r="E498" s="1"/>
+      <c r="F498" s="1"/>
+      <c r="G498" s="1"/>
+      <c r="H498" s="1"/>
+      <c r="I498" s="1"/>
+      <c r="J498" s="1"/>
+      <c r="K498" s="1"/>
+      <c r="L498" s="1"/>
+    </row>
+    <row r="499" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C499" t="s">
+        <v>85</v>
+      </c>
+      <c r="G499" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="500" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C500" s="3"/>
+      <c r="D500" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E500" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G500" s="3"/>
+      <c r="H500" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I500" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="501" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C501" s="3">
+        <v>0</v>
+      </c>
+      <c r="D501" s="3">
+        <v>0</v>
+      </c>
+      <c r="E501" s="1">
+        <f>(D501/$D$513)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G501" s="3">
+        <v>0</v>
+      </c>
+      <c r="H501" s="3">
+        <v>0</v>
+      </c>
+      <c r="I501" s="1">
+        <f>(H501/$H$511)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C502" s="3">
+        <v>1</v>
+      </c>
+      <c r="D502" s="3">
+        <v>46.153849999999998</v>
+      </c>
+      <c r="E502" s="1">
+        <f t="shared" ref="E502:E513" si="79">(D502/$D$513)*1536</f>
+        <v>59.076928000000002</v>
+      </c>
+      <c r="G502" s="3">
+        <v>1</v>
+      </c>
+      <c r="H502" s="3">
+        <v>138.46154000000001</v>
+      </c>
+      <c r="I502" s="1">
+        <f t="shared" ref="I502:I511" si="80">(H502/$H$511)*1536</f>
+        <v>177.23077120000002</v>
+      </c>
+    </row>
+    <row r="503" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C503" s="3">
+        <v>2</v>
+      </c>
+      <c r="D503" s="3">
+        <v>184.61537999999999</v>
+      </c>
+      <c r="E503" s="1">
+        <f t="shared" si="79"/>
+        <v>236.30768639999997</v>
+      </c>
+      <c r="G503" s="3">
+        <v>2</v>
+      </c>
+      <c r="H503" s="3">
+        <v>230.76922999999999</v>
+      </c>
+      <c r="I503" s="1">
+        <f t="shared" si="80"/>
+        <v>295.38461440000003</v>
+      </c>
+    </row>
+    <row r="504" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C504" s="3">
+        <v>3</v>
+      </c>
+      <c r="D504" s="3">
+        <v>230.76922999999999</v>
+      </c>
+      <c r="E504" s="1">
+        <f t="shared" si="79"/>
+        <v>295.38461440000003</v>
+      </c>
+      <c r="G504" s="3">
+        <v>3</v>
+      </c>
+      <c r="H504" s="3">
+        <v>369.23077000000001</v>
+      </c>
+      <c r="I504" s="1">
+        <f t="shared" si="80"/>
+        <v>472.61538559999997</v>
+      </c>
+    </row>
+    <row r="505" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C505" s="3">
+        <v>4</v>
+      </c>
+      <c r="D505" s="3">
+        <v>369.23077000000001</v>
+      </c>
+      <c r="E505" s="1">
+        <f t="shared" si="79"/>
+        <v>472.61538559999997</v>
+      </c>
+      <c r="G505" s="3">
+        <v>4</v>
+      </c>
+      <c r="H505" s="3">
+        <v>461.53845999999999</v>
+      </c>
+      <c r="I505" s="1">
+        <f t="shared" si="80"/>
+        <v>590.76922880000006</v>
+      </c>
+    </row>
+    <row r="506" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C506" s="3">
+        <v>5</v>
+      </c>
+      <c r="D506" s="3">
+        <v>507.69231000000002</v>
+      </c>
+      <c r="E506" s="1">
+        <f t="shared" si="79"/>
+        <v>649.84615680000002</v>
+      </c>
+      <c r="G506" s="3">
+        <v>5</v>
+      </c>
+      <c r="H506" s="3">
+        <v>600</v>
+      </c>
+      <c r="I506" s="1">
+        <f t="shared" si="80"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="507" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C507" s="3">
+        <v>6</v>
+      </c>
+      <c r="D507" s="3">
+        <v>553.84614999999997</v>
+      </c>
+      <c r="E507" s="1">
+        <f t="shared" si="79"/>
+        <v>708.92307199999993</v>
+      </c>
+      <c r="G507" s="3">
+        <v>6</v>
+      </c>
+      <c r="H507" s="3">
+        <v>738.46154000000001</v>
+      </c>
+      <c r="I507" s="1">
+        <f t="shared" si="80"/>
+        <v>945.23077119999994</v>
+      </c>
+    </row>
+    <row r="508" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C508" s="3">
+        <v>7</v>
+      </c>
+      <c r="D508" s="3">
+        <v>692.30768999999998</v>
+      </c>
+      <c r="E508" s="1">
+        <f t="shared" si="79"/>
+        <v>886.15384319999998</v>
+      </c>
+      <c r="G508" s="3">
+        <v>7</v>
+      </c>
+      <c r="H508" s="3">
+        <v>830.76922999999999</v>
+      </c>
+      <c r="I508" s="1">
+        <f t="shared" si="80"/>
+        <v>1063.3846143999999</v>
+      </c>
+    </row>
+    <row r="509" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C509" s="3">
+        <v>8</v>
+      </c>
+      <c r="D509" s="3">
+        <v>738.46154000000001</v>
+      </c>
+      <c r="E509" s="1">
+        <f t="shared" si="79"/>
+        <v>945.23077119999994</v>
+      </c>
+      <c r="G509" s="3">
+        <v>8</v>
+      </c>
+      <c r="H509" s="3">
+        <v>969.23077000000001</v>
+      </c>
+      <c r="I509" s="1">
+        <f t="shared" si="80"/>
+        <v>1240.6153856000001</v>
+      </c>
+    </row>
+    <row r="510" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C510" s="3">
+        <v>9</v>
+      </c>
+      <c r="D510">
+        <v>876.92308000000003</v>
+      </c>
+      <c r="E510" s="1">
+        <f t="shared" si="79"/>
+        <v>1122.4615423999999</v>
+      </c>
+      <c r="G510" s="3">
+        <v>9</v>
+      </c>
+      <c r="H510">
+        <v>1061.53846</v>
+      </c>
+      <c r="I510" s="1">
+        <f t="shared" si="80"/>
+        <v>1358.7692288000001</v>
+      </c>
+    </row>
+    <row r="511" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C511" s="3">
+        <v>10</v>
+      </c>
+      <c r="D511" s="3">
+        <v>923.07691999999997</v>
+      </c>
+      <c r="E511" s="1">
+        <f t="shared" si="79"/>
+        <v>1181.5384576000001</v>
+      </c>
+      <c r="G511" s="3">
+        <v>10</v>
+      </c>
+      <c r="H511" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I511" s="1">
+        <f t="shared" si="80"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="512" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C512" s="3">
+        <v>11</v>
+      </c>
+      <c r="D512">
+        <v>1061.53846</v>
+      </c>
+      <c r="E512" s="1">
+        <f t="shared" si="79"/>
+        <v>1358.7692288000001</v>
+      </c>
+    </row>
+    <row r="513" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C513" s="3">
+        <v>12</v>
+      </c>
+      <c r="D513" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E513" s="1">
+        <f t="shared" si="79"/>
+        <v>1536</v>
+      </c>
+      <c r="G513" s="1"/>
+      <c r="H513" s="1"/>
+      <c r="I513" s="1"/>
+      <c r="J513" s="1"/>
+      <c r="K513" s="1"/>
+      <c r="L513" s="1"/>
+      <c r="M513" s="1"/>
+      <c r="N513" s="1"/>
+      <c r="O513" s="1"/>
+      <c r="P513" s="1"/>
+    </row>
+    <row r="515" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C515" s="1"/>
+      <c r="D515" s="1"/>
+      <c r="E515" s="1"/>
+      <c r="F515" s="1"/>
+      <c r="G515" s="1"/>
+      <c r="H515" s="1"/>
+      <c r="I515" s="1"/>
+      <c r="J515" s="1"/>
+      <c r="K515" s="1"/>
+      <c r="L515" s="1"/>
+      <c r="M515" s="1"/>
+      <c r="N515" s="1"/>
+    </row>
+    <row r="516" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C516" t="s">
+        <v>87</v>
+      </c>
+      <c r="G516" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H516" s="3"/>
+      <c r="I516" s="1"/>
+    </row>
+    <row r="517" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C517" s="3"/>
+      <c r="D517" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E517" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G517" s="3"/>
+      <c r="H517" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I517" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="518" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C518" s="3">
+        <v>0</v>
+      </c>
+      <c r="D518" s="3">
+        <v>0</v>
+      </c>
+      <c r="E518" s="1">
+        <f>(D518/$D$529)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G518" s="3">
+        <v>0</v>
+      </c>
+      <c r="H518" s="3">
+        <v>0</v>
+      </c>
+      <c r="I518" s="1">
+        <f>(H518/$H$527)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C519" s="3">
+        <v>1</v>
+      </c>
+      <c r="D519" s="3">
+        <v>130.43477999999999</v>
+      </c>
+      <c r="E519" s="1">
+        <f t="shared" ref="E519:E529" si="81">(D519/$D$529)*1536</f>
+        <v>166.95651839999999</v>
+      </c>
+      <c r="G519" s="3">
+        <v>1</v>
+      </c>
+      <c r="H519" s="3">
+        <v>113.20755</v>
+      </c>
+      <c r="I519" s="1">
+        <f t="shared" ref="I519:I527" si="82">(H519/$H$527)*1536</f>
+        <v>144.905664</v>
+      </c>
+    </row>
+    <row r="520" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C520" s="3">
+        <v>2</v>
+      </c>
+      <c r="D520" s="3">
+        <v>260.86957000000001</v>
+      </c>
+      <c r="E520" s="1">
+        <f t="shared" si="81"/>
+        <v>333.91304960000002</v>
+      </c>
+      <c r="G520" s="3">
+        <v>2</v>
+      </c>
+      <c r="H520" s="3">
+        <v>271.69810999999999</v>
+      </c>
+      <c r="I520" s="1">
+        <f t="shared" si="82"/>
+        <v>347.77358079999999</v>
+      </c>
+    </row>
+    <row r="521" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C521" s="3">
+        <v>3</v>
+      </c>
+      <c r="D521" s="3">
+        <v>391.30435</v>
+      </c>
+      <c r="E521" s="1">
+        <f t="shared" si="81"/>
+        <v>500.86956800000002</v>
+      </c>
+      <c r="G521" s="3">
+        <v>3</v>
+      </c>
+      <c r="H521" s="3">
+        <v>384.90566000000001</v>
+      </c>
+      <c r="I521" s="1">
+        <f t="shared" si="82"/>
+        <v>492.67924479999999</v>
+      </c>
+    </row>
+    <row r="522" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C522" s="3">
+        <v>4</v>
+      </c>
+      <c r="D522" s="3">
+        <v>443.47825999999998</v>
+      </c>
+      <c r="E522" s="1">
+        <f t="shared" si="81"/>
+        <v>567.65217280000002</v>
+      </c>
+      <c r="G522" s="3">
+        <v>4</v>
+      </c>
+      <c r="H522" s="3">
+        <v>543.39622999999995</v>
+      </c>
+      <c r="I522" s="1">
+        <f t="shared" si="82"/>
+        <v>695.5471743999999</v>
+      </c>
+    </row>
+    <row r="523" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C523" s="3">
+        <v>5</v>
+      </c>
+      <c r="D523" s="3">
+        <v>573.91304000000002</v>
+      </c>
+      <c r="E523" s="1">
+        <f t="shared" si="81"/>
+        <v>734.60869120000007</v>
+      </c>
+      <c r="G523" s="3">
+        <v>5</v>
+      </c>
+      <c r="H523" s="3">
+        <v>656.60377000000005</v>
+      </c>
+      <c r="I523" s="1">
+        <f t="shared" si="82"/>
+        <v>840.4528256000001</v>
+      </c>
+    </row>
+    <row r="524" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C524" s="3">
+        <v>6</v>
+      </c>
+      <c r="D524" s="3">
+        <v>704.34783000000004</v>
+      </c>
+      <c r="E524" s="1">
+        <f t="shared" si="81"/>
+        <v>901.56522240000004</v>
+      </c>
+      <c r="G524" s="3">
+        <v>6</v>
+      </c>
+      <c r="H524" s="3">
+        <v>815.09433999999999</v>
+      </c>
+      <c r="I524" s="1">
+        <f t="shared" si="82"/>
+        <v>1043.3207551999999</v>
+      </c>
+    </row>
+    <row r="525" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C525" s="3">
+        <v>7</v>
+      </c>
+      <c r="D525" s="3">
+        <v>834.78260999999998</v>
+      </c>
+      <c r="E525" s="1">
+        <f t="shared" si="81"/>
+        <v>1068.5217407999999</v>
+      </c>
+      <c r="G525" s="3">
+        <v>7</v>
+      </c>
+      <c r="H525" s="3">
+        <v>928.30188999999996</v>
+      </c>
+      <c r="I525" s="1">
+        <f t="shared" si="82"/>
+        <v>1188.2264191999998</v>
+      </c>
+    </row>
+    <row r="526" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C526" s="3">
+        <v>8</v>
+      </c>
+      <c r="D526" s="3">
+        <v>886.95651999999995</v>
+      </c>
+      <c r="E526" s="1">
+        <f t="shared" si="81"/>
+        <v>1135.3043456</v>
+      </c>
+      <c r="G526" s="3">
+        <v>8</v>
+      </c>
+      <c r="H526">
+        <v>1086.7924499999999</v>
+      </c>
+      <c r="I526" s="1">
+        <f t="shared" si="82"/>
+        <v>1391.0943359999999</v>
+      </c>
+    </row>
+    <row r="527" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C527" s="3">
+        <v>9</v>
+      </c>
+      <c r="D527">
+        <v>1017.3913</v>
+      </c>
+      <c r="E527" s="1">
+        <f t="shared" si="81"/>
+        <v>1302.2608639999999</v>
+      </c>
+      <c r="G527" s="3">
+        <v>9</v>
+      </c>
+      <c r="H527" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I527" s="1">
+        <f t="shared" si="82"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="528" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C528" s="3">
+        <v>10</v>
+      </c>
+      <c r="D528" s="3">
+        <v>1147.82609</v>
+      </c>
+      <c r="E528" s="1">
+        <f t="shared" si="81"/>
+        <v>1469.2173952000001</v>
+      </c>
+    </row>
+    <row r="529" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C529" s="3">
+        <v>11</v>
+      </c>
+      <c r="D529">
+        <v>1200</v>
+      </c>
+      <c r="E529" s="1">
+        <f t="shared" si="81"/>
+        <v>1536</v>
+      </c>
+      <c r="G529" s="1"/>
+      <c r="H529" s="1"/>
+      <c r="I529" s="1"/>
+      <c r="J529" s="1"/>
+      <c r="K529" s="1"/>
+      <c r="L529" s="1"/>
+      <c r="M529" s="1"/>
+      <c r="N529" s="1"/>
+      <c r="O529" s="1"/>
+    </row>
+    <row r="531" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C531" s="1"/>
+      <c r="D531" s="1"/>
+      <c r="E531" s="1"/>
+      <c r="F531" s="1"/>
+      <c r="G531" s="1"/>
+      <c r="H531" s="1"/>
+      <c r="I531" s="1"/>
+      <c r="J531" s="1"/>
+      <c r="K531" s="1"/>
+      <c r="L531" s="1"/>
+      <c r="M531" s="1"/>
+    </row>
+    <row r="533" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C533" t="s">
+        <v>89</v>
+      </c>
+      <c r="G533" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H533" s="3"/>
+      <c r="I533" s="1"/>
+    </row>
+    <row r="534" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C534" s="3"/>
+      <c r="D534" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E534" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G534" s="3"/>
+      <c r="H534" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I534" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="535" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C535" s="3">
+        <v>0</v>
+      </c>
+      <c r="D535" s="3">
+        <v>0</v>
+      </c>
+      <c r="E535" s="1">
+        <f>(D535/$D$547)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G535" s="3">
+        <v>0</v>
+      </c>
+      <c r="H535" s="3">
+        <v>0</v>
+      </c>
+      <c r="I535" s="1">
+        <f>(H535/$H$542)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C536" s="3">
+        <v>1</v>
+      </c>
+      <c r="D536" s="3">
+        <v>200</v>
+      </c>
+      <c r="E536" s="1">
+        <f t="shared" ref="E536:E547" si="83">(D536/$D$547)*1536</f>
+        <v>256</v>
+      </c>
+      <c r="G536" s="3">
+        <v>1</v>
+      </c>
+      <c r="H536" s="3">
+        <v>157.57576</v>
+      </c>
+      <c r="I536" s="1">
+        <f t="shared" ref="I536:I542" si="84">(H536/$H$542)*1536</f>
+        <v>201.6969728</v>
+      </c>
+    </row>
+    <row r="537" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C537" s="3">
+        <v>2</v>
+      </c>
+      <c r="D537" s="3">
+        <v>266.66699999999997</v>
+      </c>
+      <c r="E537" s="1">
+        <f t="shared" si="83"/>
+        <v>341.33375999999998</v>
+      </c>
+      <c r="G537" s="3">
+        <v>2</v>
+      </c>
+      <c r="H537" s="3">
+        <v>387.87878999999998</v>
+      </c>
+      <c r="I537" s="1">
+        <f t="shared" si="84"/>
+        <v>496.48485119999998</v>
+      </c>
+    </row>
+    <row r="538" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C538" s="3">
+        <v>3</v>
+      </c>
+      <c r="D538" s="3">
+        <v>383.33300000000003</v>
+      </c>
+      <c r="E538" s="1">
+        <f t="shared" si="83"/>
+        <v>490.66624000000002</v>
+      </c>
+      <c r="G538" s="3">
+        <v>3</v>
+      </c>
+      <c r="H538" s="3">
+        <v>545.45455000000004</v>
+      </c>
+      <c r="I538" s="1">
+        <f t="shared" si="84"/>
+        <v>698.18182400000001</v>
+      </c>
+    </row>
+    <row r="539" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C539" s="3">
+        <v>4</v>
+      </c>
+      <c r="D539" s="3">
+        <v>433.33300000000003</v>
+      </c>
+      <c r="E539" s="1">
+        <f t="shared" si="83"/>
+        <v>554.66624000000002</v>
+      </c>
+      <c r="G539" s="3">
+        <v>4</v>
+      </c>
+      <c r="H539" s="3">
+        <v>703.03030000000001</v>
+      </c>
+      <c r="I539" s="1">
+        <f t="shared" si="84"/>
+        <v>899.878784</v>
+      </c>
+    </row>
+    <row r="540" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C540" s="3">
+        <v>5</v>
+      </c>
+      <c r="D540" s="3">
+        <v>500</v>
+      </c>
+      <c r="E540" s="1">
+        <f t="shared" si="83"/>
+        <v>640</v>
+      </c>
+      <c r="G540" s="3">
+        <v>5</v>
+      </c>
+      <c r="H540" s="3">
+        <v>933.33333000000005</v>
+      </c>
+      <c r="I540" s="1">
+        <f t="shared" si="84"/>
+        <v>1194.6666624</v>
+      </c>
+    </row>
+    <row r="541" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C541" s="3">
+        <v>6</v>
+      </c>
+      <c r="D541" s="3">
+        <v>550</v>
+      </c>
+      <c r="E541" s="1">
+        <f t="shared" si="83"/>
+        <v>704</v>
+      </c>
+      <c r="G541" s="3">
+        <v>6</v>
+      </c>
+      <c r="H541" s="3">
+        <v>1090.9090900000001</v>
+      </c>
+      <c r="I541" s="1">
+        <f t="shared" si="84"/>
+        <v>1396.3636352000001</v>
+      </c>
+    </row>
+    <row r="542" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C542" s="3">
+        <v>7</v>
+      </c>
+      <c r="D542" s="3">
+        <v>700</v>
+      </c>
+      <c r="E542" s="1">
+        <f t="shared" si="83"/>
+        <v>896</v>
+      </c>
+      <c r="G542" s="3">
+        <v>7</v>
+      </c>
+      <c r="H542" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I542" s="1">
+        <f t="shared" si="84"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="543" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C543" s="3">
+        <v>8</v>
+      </c>
+      <c r="D543" s="3">
+        <v>883.33299999999997</v>
+      </c>
+      <c r="E543" s="1">
+        <f t="shared" si="83"/>
+        <v>1130.66624</v>
+      </c>
+    </row>
+    <row r="544" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C544" s="3">
+        <v>9</v>
+      </c>
+      <c r="D544">
+        <v>966.66700000000003</v>
+      </c>
+      <c r="E544" s="1">
+        <f t="shared" si="83"/>
+        <v>1237.33376</v>
+      </c>
+      <c r="G544" s="1"/>
+      <c r="H544" s="1"/>
+      <c r="I544" s="1"/>
+      <c r="J544" s="1"/>
+      <c r="K544" s="1"/>
+      <c r="L544" s="1"/>
+      <c r="M544" s="1"/>
+    </row>
+    <row r="545" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C545" s="3">
+        <v>10</v>
+      </c>
+      <c r="D545" s="3">
+        <v>1050</v>
+      </c>
+      <c r="E545" s="1">
+        <f t="shared" si="83"/>
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="546" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C546" s="3">
+        <v>11</v>
+      </c>
+      <c r="D546">
+        <v>1083.3330000000001</v>
+      </c>
+      <c r="E546" s="1">
+        <f t="shared" si="83"/>
+        <v>1386.6662400000002</v>
+      </c>
+    </row>
+    <row r="547" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C547" s="3">
+        <v>12</v>
+      </c>
+      <c r="D547" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E547" s="1">
+        <f t="shared" si="83"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="548" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C548" s="1"/>
+      <c r="D548" s="1"/>
+      <c r="E548" s="1"/>
+      <c r="F548" s="1"/>
+      <c r="G548" s="1"/>
+      <c r="H548" s="1"/>
+      <c r="I548" s="1"/>
+      <c r="J548" s="1"/>
+      <c r="K548" s="1"/>
+      <c r="L548" s="1"/>
+      <c r="M548" s="1"/>
+      <c r="N548" s="1"/>
+    </row>
+    <row r="550" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C550" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D550" s="3"/>
+      <c r="E550" s="1"/>
+      <c r="G550" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H550" s="3"/>
+      <c r="I550" s="1"/>
+    </row>
+    <row r="551" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C551" s="3"/>
+      <c r="D551" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E551" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G551" s="3"/>
+      <c r="H551" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I551" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="552" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C552" s="3">
+        <v>0</v>
+      </c>
+      <c r="D552" s="3">
+        <v>0</v>
+      </c>
+      <c r="E552" s="1">
+        <f>(D552/$D$560)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G552" s="3">
+        <v>0</v>
+      </c>
+      <c r="H552" s="3">
+        <v>0</v>
+      </c>
+      <c r="I552" s="1">
+        <f>(H552/$H$561)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C553" s="3">
+        <v>1</v>
+      </c>
+      <c r="D553" s="3">
+        <v>118.81188</v>
+      </c>
+      <c r="E553" s="1">
+        <f t="shared" ref="E553:E560" si="85">(D553/$D$560)*1536</f>
+        <v>152.0792064</v>
+      </c>
+      <c r="G553" s="3">
+        <v>1</v>
+      </c>
+      <c r="H553" s="3">
+        <v>203.19488999999999</v>
+      </c>
+      <c r="I553" s="1">
+        <f t="shared" ref="I553:I561" si="86">(H553/$H$561)*1536</f>
+        <v>260.08945919999996</v>
+      </c>
+    </row>
+    <row r="554" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C554" s="3">
+        <v>2</v>
+      </c>
+      <c r="D554" s="3">
+        <v>350.49504999999999</v>
+      </c>
+      <c r="E554" s="1">
+        <f t="shared" si="85"/>
+        <v>448.63366400000001</v>
+      </c>
+      <c r="G554" s="3">
+        <v>2</v>
+      </c>
+      <c r="H554" s="3">
+        <v>249.20128</v>
+      </c>
+      <c r="I554" s="1">
+        <f t="shared" si="86"/>
+        <v>318.97763839999999</v>
+      </c>
+    </row>
+    <row r="555" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C555" s="3">
+        <v>3</v>
+      </c>
+      <c r="D555" s="3">
+        <v>386.13861000000003</v>
+      </c>
+      <c r="E555" s="1">
+        <f t="shared" si="85"/>
+        <v>494.25742079999998</v>
+      </c>
+      <c r="G555" s="3">
+        <v>3</v>
+      </c>
+      <c r="H555" s="3">
+        <v>452.39616999999998</v>
+      </c>
+      <c r="I555" s="1">
+        <f t="shared" si="86"/>
+        <v>579.06709760000001</v>
+      </c>
+    </row>
+    <row r="556" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C556" s="3">
+        <v>4</v>
+      </c>
+      <c r="D556" s="3">
+        <v>617.82177999999999</v>
+      </c>
+      <c r="E556" s="1">
+        <f t="shared" si="85"/>
+        <v>790.81187839999996</v>
+      </c>
+      <c r="G556" s="3">
+        <v>4</v>
+      </c>
+      <c r="H556" s="3">
+        <v>498.40255999999999</v>
+      </c>
+      <c r="I556" s="1">
+        <f t="shared" si="86"/>
+        <v>637.95527679999998</v>
+      </c>
+    </row>
+    <row r="557" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C557" s="3">
+        <v>5</v>
+      </c>
+      <c r="D557" s="3">
+        <v>700.99009999999998</v>
+      </c>
+      <c r="E557" s="1">
+        <f t="shared" si="85"/>
+        <v>897.26732800000002</v>
+      </c>
+      <c r="G557" s="3">
+        <v>5</v>
+      </c>
+      <c r="H557" s="3">
+        <v>701.59744000000001</v>
+      </c>
+      <c r="I557" s="1">
+        <f t="shared" si="86"/>
+        <v>898.04472320000002</v>
+      </c>
+    </row>
+    <row r="558" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C558" s="3">
+        <v>6</v>
+      </c>
+      <c r="D558" s="3">
+        <v>932.67327</v>
+      </c>
+      <c r="E558" s="1">
+        <f t="shared" si="85"/>
+        <v>1193.8217856000001</v>
+      </c>
+      <c r="G558" s="3">
+        <v>6</v>
+      </c>
+      <c r="H558" s="3">
+        <v>747.60383000000002</v>
+      </c>
+      <c r="I558" s="1">
+        <f t="shared" si="86"/>
+        <v>956.9329024000001</v>
+      </c>
+    </row>
+    <row r="559" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C559" s="3">
+        <v>7</v>
+      </c>
+      <c r="D559" s="3">
+        <v>968.31682999999998</v>
+      </c>
+      <c r="E559" s="1">
+        <f t="shared" si="85"/>
+        <v>1239.4455424</v>
+      </c>
+      <c r="G559" s="3">
+        <v>7</v>
+      </c>
+      <c r="H559" s="3">
+        <v>950.79872</v>
+      </c>
+      <c r="I559" s="1">
+        <f t="shared" si="86"/>
+        <v>1217.0223616000001</v>
+      </c>
+    </row>
+    <row r="560" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C560" s="3">
+        <v>8</v>
+      </c>
+      <c r="D560" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E560" s="1">
+        <f t="shared" si="85"/>
+        <v>1536</v>
+      </c>
+      <c r="G560" s="3">
+        <v>8</v>
+      </c>
+      <c r="H560">
+        <v>996.80511000000001</v>
+      </c>
+      <c r="I560" s="1">
+        <f t="shared" si="86"/>
+        <v>1275.9105408</v>
+      </c>
+    </row>
+    <row r="561" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="G561" s="3">
+        <v>9</v>
+      </c>
+      <c r="H561" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I561" s="1">
+        <f t="shared" si="86"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="562" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C562" s="1"/>
+      <c r="D562" s="1"/>
+      <c r="E562" s="1"/>
+      <c r="F562" s="1"/>
+      <c r="G562" s="1"/>
+      <c r="H562" s="1"/>
+      <c r="I562" s="1"/>
+      <c r="J562" s="1"/>
+      <c r="K562" s="1"/>
+      <c r="L562" s="1"/>
+      <c r="M562" s="1"/>
+      <c r="N562" s="1"/>
+      <c r="O562" s="1"/>
+    </row>
+    <row r="564" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C564" t="s">
+        <v>92</v>
+      </c>
+      <c r="G564" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="565" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C565" s="3"/>
+      <c r="D565" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E565" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G565" s="3"/>
+      <c r="H565" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I565" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="566" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C566" s="3">
+        <v>0</v>
+      </c>
+      <c r="D566" s="3">
+        <v>0</v>
+      </c>
+      <c r="E566" s="1">
+        <f>(D566/$D$578)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G566" s="3">
+        <v>0</v>
+      </c>
+      <c r="H566" s="3">
+        <v>0</v>
+      </c>
+      <c r="I566" s="1">
+        <f>(H566/$H$578)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="567" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C567" s="3">
+        <v>1</v>
+      </c>
+      <c r="D567" s="3">
+        <v>49.415390000000002</v>
+      </c>
+      <c r="E567" s="1">
+        <f t="shared" ref="E567:E578" si="87">(D567/$D$578)*1536</f>
+        <v>63.251699200000004</v>
+      </c>
+      <c r="G567" s="3">
+        <v>1</v>
+      </c>
+      <c r="H567" s="3">
+        <v>58.236040000000003</v>
+      </c>
+      <c r="I567" s="1">
+        <f t="shared" ref="I567:I578" si="88">(H567/$H$578)*1536</f>
+        <v>74.572837808848433</v>
+      </c>
+    </row>
+    <row r="568" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C568" s="3">
+        <v>2</v>
+      </c>
+      <c r="D568" s="3">
+        <v>232.46054000000001</v>
+      </c>
+      <c r="E568" s="1">
+        <f t="shared" si="87"/>
+        <v>297.54949119999998</v>
+      </c>
+      <c r="G568" s="3">
+        <v>2</v>
+      </c>
+      <c r="H568" s="3">
+        <v>206.95866000000001</v>
+      </c>
+      <c r="I568" s="1">
+        <f t="shared" si="88"/>
+        <v>265.01620964125664</v>
+      </c>
+    </row>
+    <row r="569" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C569" s="3">
+        <v>3</v>
+      </c>
+      <c r="D569" s="3">
+        <v>316.92773</v>
+      </c>
+      <c r="E569" s="1">
+        <f t="shared" si="87"/>
+        <v>405.66749440000001</v>
+      </c>
+      <c r="G569" s="3">
+        <v>3</v>
+      </c>
+      <c r="H569" s="3">
+        <v>265.19470999999999</v>
+      </c>
+      <c r="I569" s="1">
+        <f t="shared" si="88"/>
+        <v>339.58906025537783</v>
+      </c>
+    </row>
+    <row r="570" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C570" s="3">
+        <v>4</v>
+      </c>
+      <c r="D570" s="3">
+        <v>383.74261000000001</v>
+      </c>
+      <c r="E570" s="1">
+        <f t="shared" si="87"/>
+        <v>491.19054080000001</v>
+      </c>
+      <c r="G570" s="3">
+        <v>4</v>
+      </c>
+      <c r="H570" s="3">
+        <v>413.91732999999999</v>
+      </c>
+      <c r="I570" s="1">
+        <f t="shared" si="88"/>
+        <v>530.03243208778599</v>
+      </c>
+    </row>
+    <row r="571" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C571" s="3">
+        <v>5</v>
+      </c>
+      <c r="D571" s="3">
+        <v>549.38827000000003</v>
+      </c>
+      <c r="E571" s="1">
+        <f t="shared" si="87"/>
+        <v>703.21698560000004</v>
+      </c>
+      <c r="G571" s="3">
+        <v>5</v>
+      </c>
+      <c r="H571" s="3">
+        <v>472.15337</v>
+      </c>
+      <c r="I571" s="1">
+        <f t="shared" si="88"/>
+        <v>604.60526989663447</v>
+      </c>
+    </row>
+    <row r="572" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C572" s="3">
+        <v>6</v>
+      </c>
+      <c r="D572" s="3">
+        <v>616.20315000000005</v>
+      </c>
+      <c r="E572" s="1">
+        <f t="shared" si="87"/>
+        <v>788.74003199999993</v>
+      </c>
+      <c r="G572" s="3">
+        <v>6</v>
+      </c>
+      <c r="H572" s="3">
+        <v>554.50964999999997</v>
+      </c>
+      <c r="I572" s="1">
+        <f t="shared" si="88"/>
+        <v>710.06473298822016</v>
+      </c>
+    </row>
+    <row r="573" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C573" s="3">
+        <v>7</v>
+      </c>
+      <c r="D573" s="3">
+        <v>700.67034000000001</v>
+      </c>
+      <c r="E573" s="1">
+        <f t="shared" si="87"/>
+        <v>896.85803520000013</v>
+      </c>
+      <c r="G573" s="3">
+        <v>7</v>
+      </c>
+      <c r="H573" s="3">
+        <v>703.23226999999997</v>
+      </c>
+      <c r="I573" s="1">
+        <f t="shared" si="88"/>
+        <v>900.50810482062832</v>
+      </c>
+    </row>
+    <row r="574" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C574" s="3">
+        <v>8</v>
+      </c>
+      <c r="D574" s="3">
+        <v>883.71549000000005</v>
+      </c>
+      <c r="E574" s="1">
+        <f t="shared" si="87"/>
+        <v>1131.1558272000002</v>
+      </c>
+      <c r="G574" s="3">
+        <v>8</v>
+      </c>
+      <c r="H574" s="3">
+        <v>761.46831999999995</v>
+      </c>
+      <c r="I574" s="1">
+        <f t="shared" si="88"/>
+        <v>975.08095543474951</v>
+      </c>
+    </row>
+    <row r="575" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C575" s="3">
+        <v>9</v>
+      </c>
+      <c r="D575">
+        <v>933.13088000000005</v>
+      </c>
+      <c r="E575" s="1">
+        <f t="shared" si="87"/>
+        <v>1194.4075264000001</v>
+      </c>
+      <c r="G575" s="3">
+        <v>9</v>
+      </c>
+      <c r="H575">
+        <v>910.19093999999996</v>
+      </c>
+      <c r="I575" s="1">
+        <f t="shared" si="88"/>
+        <v>1165.5243272671578</v>
+      </c>
+    </row>
+    <row r="576" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C576" s="3">
+        <v>10</v>
+      </c>
+      <c r="D576" s="3">
+        <v>968.18268</v>
+      </c>
+      <c r="E576" s="1">
+        <f t="shared" si="87"/>
+        <v>1239.2738304</v>
+      </c>
+      <c r="G576" s="3">
+        <v>10</v>
+      </c>
+      <c r="H576" s="3">
+        <v>968.42697999999996</v>
+      </c>
+      <c r="I576" s="1">
+        <f t="shared" si="88"/>
+        <v>1240.0971650760061</v>
+      </c>
+    </row>
+    <row r="577" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C577" s="3">
+        <v>11</v>
+      </c>
+      <c r="D577">
+        <v>1165.59142</v>
+      </c>
+      <c r="E577" s="1">
+        <f t="shared" si="87"/>
+        <v>1491.9570176</v>
+      </c>
+      <c r="G577" s="3">
+        <v>11</v>
+      </c>
+      <c r="H577">
+        <v>1117.1496</v>
+      </c>
+      <c r="I577" s="1">
+        <f t="shared" si="88"/>
+        <v>1430.5405369084144</v>
+      </c>
+    </row>
+    <row r="578" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C578" s="3">
+        <v>12</v>
+      </c>
+      <c r="D578" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E578" s="1">
+        <f t="shared" si="87"/>
+        <v>1536</v>
+      </c>
+      <c r="G578" s="3">
+        <v>12</v>
+      </c>
+      <c r="H578" s="3">
+        <v>1199.5058799999999</v>
+      </c>
+      <c r="I578" s="1">
+        <f t="shared" si="88"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="579" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C579" s="1"/>
+      <c r="D579" s="1"/>
+      <c r="E579" s="1"/>
+      <c r="F579" s="1"/>
+      <c r="G579" s="1"/>
+      <c r="H579" s="1"/>
+      <c r="I579" s="1"/>
+      <c r="J579" s="1"/>
+      <c r="K579" s="1"/>
+      <c r="L579" s="1"/>
+      <c r="M579" s="1"/>
+      <c r="N579" s="1"/>
+      <c r="O579" s="1"/>
+      <c r="P579" s="1"/>
+      <c r="Q579" s="1"/>
+      <c r="R579" s="1"/>
+    </row>
+    <row r="581" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C581" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D581" s="3"/>
+      <c r="E581" s="1"/>
+      <c r="G581" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H581" s="3"/>
+      <c r="I581" s="1"/>
+    </row>
+    <row r="582" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C582" s="3"/>
+      <c r="D582" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E582" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G582" s="3"/>
+      <c r="H582" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I582" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="583" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C583" s="3">
+        <v>0</v>
+      </c>
+      <c r="D583" s="3">
+        <v>0</v>
+      </c>
+      <c r="E583" s="1">
+        <f>(D583/$D$588)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G583" s="3">
+        <v>0</v>
+      </c>
+      <c r="H583" s="3">
+        <v>0</v>
+      </c>
+      <c r="I583" s="1">
+        <f>(H583/$H$590)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C584" s="3">
+        <v>1</v>
+      </c>
+      <c r="D584" s="3">
+        <v>185</v>
+      </c>
+      <c r="E584" s="1">
+        <f t="shared" ref="E584:E588" si="89">(D584/$D$588)*1536</f>
+        <v>236.8</v>
+      </c>
+      <c r="G584" s="3">
+        <v>1</v>
+      </c>
+      <c r="H584" s="3">
+        <v>197</v>
+      </c>
+      <c r="I584" s="1">
+        <f t="shared" ref="I584:I590" si="90">(H584/$H$590)*1536</f>
+        <v>252.15999999999997</v>
+      </c>
+    </row>
+    <row r="585" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C585" s="3">
+        <v>2</v>
+      </c>
+      <c r="D585" s="3">
+        <v>337</v>
+      </c>
+      <c r="E585" s="1">
+        <f t="shared" si="89"/>
+        <v>431.36</v>
+      </c>
+      <c r="G585" s="3">
+        <v>2</v>
+      </c>
+      <c r="H585" s="3">
+        <v>341</v>
+      </c>
+      <c r="I585" s="1">
+        <f t="shared" si="90"/>
+        <v>436.48</v>
+      </c>
+    </row>
+    <row r="586" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C586" s="3">
+        <v>3</v>
+      </c>
+      <c r="D586" s="3">
+        <v>683</v>
+      </c>
+      <c r="E586" s="1">
+        <f t="shared" si="89"/>
+        <v>874.24</v>
+      </c>
+      <c r="G586" s="3">
+        <v>3</v>
+      </c>
+      <c r="H586" s="3">
+        <v>495</v>
+      </c>
+      <c r="I586" s="1">
+        <f t="shared" si="90"/>
+        <v>633.59999999999991</v>
+      </c>
+    </row>
+    <row r="587" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C587" s="3">
+        <v>4</v>
+      </c>
+      <c r="D587" s="3">
+        <v>790</v>
+      </c>
+      <c r="E587" s="1">
+        <f t="shared" si="89"/>
+        <v>1011.2</v>
+      </c>
+      <c r="G587" s="3">
+        <v>4</v>
+      </c>
+      <c r="H587" s="3">
+        <v>703</v>
+      </c>
+      <c r="I587" s="1">
+        <f t="shared" si="90"/>
+        <v>899.83999999999992</v>
+      </c>
+    </row>
+    <row r="588" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C588" s="3">
+        <v>5</v>
+      </c>
+      <c r="D588" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E588" s="1">
+        <f t="shared" si="89"/>
+        <v>1536</v>
+      </c>
+      <c r="G588" s="3">
+        <v>5</v>
+      </c>
+      <c r="H588" s="3">
+        <v>853</v>
+      </c>
+      <c r="I588" s="1">
+        <f t="shared" si="90"/>
+        <v>1091.8399999999999</v>
+      </c>
+    </row>
+    <row r="589" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C589" s="3"/>
+      <c r="D589" s="3"/>
+      <c r="E589" s="1"/>
+      <c r="G589" s="3">
+        <v>6</v>
+      </c>
+      <c r="H589" s="3">
+        <v>1009</v>
+      </c>
+      <c r="I589" s="1">
+        <f t="shared" si="90"/>
+        <v>1291.52</v>
+      </c>
+    </row>
+    <row r="590" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C590" s="3"/>
+      <c r="D590" s="3"/>
+      <c r="E590" s="1"/>
+      <c r="G590" s="3">
+        <v>7</v>
+      </c>
+      <c r="H590" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I590" s="1">
+        <f t="shared" si="90"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="593" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C593" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D593" s="3"/>
+      <c r="E593" s="1"/>
+      <c r="G593" t="s">
+        <v>97</v>
+      </c>
+      <c r="I593" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="594" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C594" s="3"/>
+      <c r="D594" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E594" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G594" s="3"/>
+      <c r="H594" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I594" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="595" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C595" s="3">
+        <v>0</v>
+      </c>
+      <c r="D595" s="3">
+        <v>0</v>
+      </c>
+      <c r="E595" s="1">
+        <f>(D595/$D$602)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G595" s="3">
+        <v>0</v>
+      </c>
+      <c r="H595" s="3">
+        <v>0</v>
+      </c>
+      <c r="I595" s="1">
+        <f>(H595/$H$607)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="596" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C596" s="3">
+        <v>1</v>
+      </c>
+      <c r="D596" s="3">
+        <v>161</v>
+      </c>
+      <c r="E596" s="1">
+        <f t="shared" ref="E596:E602" si="91">(D596/$D$602)*1536</f>
+        <v>206.07999999999998</v>
+      </c>
+      <c r="G596" s="3">
+        <v>1</v>
+      </c>
+      <c r="H596" s="3">
+        <v>94.135000000000005</v>
+      </c>
+      <c r="I596" s="1">
+        <f t="shared" ref="I596:I607" si="92">(H596/$H$607)*1536</f>
+        <v>120.49280000000002</v>
+      </c>
+    </row>
+    <row r="597" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C597" s="3">
+        <v>2</v>
+      </c>
+      <c r="D597" s="3">
+        <v>346</v>
+      </c>
+      <c r="E597" s="1">
+        <f t="shared" si="91"/>
+        <v>442.88</v>
+      </c>
+      <c r="G597" s="3">
+        <v>2</v>
+      </c>
+      <c r="H597" s="3">
+        <v>196.09</v>
+      </c>
+      <c r="I597" s="1">
+        <f t="shared" si="92"/>
+        <v>250.99520000000001</v>
+      </c>
+    </row>
+    <row r="598" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C598" s="3">
+        <v>3</v>
+      </c>
+      <c r="D598" s="3">
+        <v>526</v>
+      </c>
+      <c r="E598" s="1">
+        <f t="shared" si="91"/>
+        <v>673.28</v>
+      </c>
+      <c r="G598" s="3">
+        <v>3</v>
+      </c>
+      <c r="H598" s="3">
+        <v>298.04500000000002</v>
+      </c>
+      <c r="I598" s="1">
+        <f t="shared" si="92"/>
+        <v>381.49760000000003</v>
+      </c>
+    </row>
+    <row r="599" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C599" s="3">
+        <v>4</v>
+      </c>
+      <c r="D599" s="3">
+        <v>686</v>
+      </c>
+      <c r="E599" s="1">
+        <f t="shared" si="91"/>
+        <v>878.07999999999993</v>
+      </c>
+      <c r="G599" s="3">
+        <v>4</v>
+      </c>
+      <c r="H599" s="3">
+        <v>392.18</v>
+      </c>
+      <c r="I599" s="1">
+        <f t="shared" si="92"/>
+        <v>501.99040000000002</v>
+      </c>
+    </row>
+    <row r="600" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C600" s="3">
+        <v>5</v>
+      </c>
+      <c r="D600" s="3">
+        <v>862</v>
+      </c>
+      <c r="E600" s="1">
+        <f t="shared" si="91"/>
+        <v>1103.3600000000001</v>
+      </c>
+      <c r="G600" s="3">
+        <v>5</v>
+      </c>
+      <c r="H600" s="3">
+        <v>501.95499999999998</v>
+      </c>
+      <c r="I600" s="1">
+        <f t="shared" si="92"/>
+        <v>642.50239999999997</v>
+      </c>
+    </row>
+    <row r="601" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C601" s="3">
+        <v>6</v>
+      </c>
+      <c r="D601" s="3">
+        <v>1028.5709999999999</v>
+      </c>
+      <c r="E601" s="1">
+        <f t="shared" si="91"/>
+        <v>1316.5708799999998</v>
+      </c>
+      <c r="G601" s="3">
+        <v>6</v>
+      </c>
+      <c r="H601" s="3">
+        <v>592.17999999999995</v>
+      </c>
+      <c r="I601" s="1">
+        <f t="shared" si="92"/>
+        <v>757.99039999999991</v>
+      </c>
+    </row>
+    <row r="602" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C602" s="3">
+        <v>7</v>
+      </c>
+      <c r="D602" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E602" s="1">
+        <f t="shared" si="91"/>
+        <v>1536</v>
+      </c>
+      <c r="G602" s="3">
+        <v>7</v>
+      </c>
+      <c r="H602" s="3">
+        <v>698.04499999999996</v>
+      </c>
+      <c r="I602" s="1">
+        <f t="shared" si="92"/>
+        <v>893.49759999999992</v>
+      </c>
+    </row>
+    <row r="603" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G603" s="3">
+        <v>8</v>
+      </c>
+      <c r="H603" s="3">
+        <v>796.09</v>
+      </c>
+      <c r="I603" s="1">
+        <f t="shared" si="92"/>
+        <v>1018.9952000000001</v>
+      </c>
+    </row>
+    <row r="604" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G604" s="3">
+        <v>9</v>
+      </c>
+      <c r="H604">
+        <v>894.13499999999999</v>
+      </c>
+      <c r="I604" s="1">
+        <f t="shared" si="92"/>
+        <v>1144.4928</v>
+      </c>
+    </row>
+    <row r="605" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G605" s="3">
+        <v>10</v>
+      </c>
+      <c r="H605" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I605" s="1">
+        <f t="shared" si="92"/>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="606" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G606" s="3">
+        <v>11</v>
+      </c>
+      <c r="H606">
+        <v>1090.2249999999999</v>
+      </c>
+      <c r="I606" s="1">
+        <f t="shared" si="92"/>
+        <v>1395.4879999999998</v>
+      </c>
+    </row>
+    <row r="607" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="G607" s="3">
+        <v>12</v>
+      </c>
+      <c r="H607" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I607" s="1">
+        <f t="shared" si="92"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="610" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C610" t="s">
+        <v>98</v>
+      </c>
+      <c r="F610" t="s">
+        <v>103</v>
+      </c>
+      <c r="G610" t="s">
+        <v>99</v>
+      </c>
+      <c r="J610" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="611" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C611" s="3"/>
+      <c r="D611" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E611" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G611" s="3"/>
+      <c r="H611" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I611" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="612" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C612" s="3">
+        <v>0</v>
+      </c>
+      <c r="D612" s="3">
+        <v>0</v>
+      </c>
+      <c r="E612" s="1">
+        <f>(D612/$D$625)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G612" s="3">
+        <v>0</v>
+      </c>
+      <c r="H612" s="3">
+        <v>0</v>
+      </c>
+      <c r="I612" s="1">
+        <f>(H612/$H$625)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C613" s="3">
+        <v>1</v>
+      </c>
+      <c r="D613" s="3">
+        <v>109.09090999999999</v>
+      </c>
+      <c r="E613" s="1">
+        <f t="shared" ref="E613:E625" si="93">(D613/$D$625)*1536</f>
+        <v>139.6363648</v>
+      </c>
+      <c r="G613" s="3">
+        <v>1</v>
+      </c>
+      <c r="H613" s="3">
+        <v>126.31579000000001</v>
+      </c>
+      <c r="I613" s="1">
+        <f t="shared" ref="I613:I625" si="94">(H613/$H$625)*1536</f>
+        <v>161.68421120000002</v>
+      </c>
+    </row>
+    <row r="614" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C614" s="3">
+        <v>2</v>
+      </c>
+      <c r="D614" s="3">
+        <v>218.18181999999999</v>
+      </c>
+      <c r="E614" s="1">
+        <f t="shared" si="93"/>
+        <v>279.27272959999999</v>
+      </c>
+      <c r="G614" s="3">
+        <v>2</v>
+      </c>
+      <c r="H614" s="3">
+        <v>189.47368</v>
+      </c>
+      <c r="I614" s="1">
+        <f t="shared" si="94"/>
+        <v>242.5263104</v>
+      </c>
+    </row>
+    <row r="615" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C615" s="3">
+        <v>3</v>
+      </c>
+      <c r="D615" s="3">
+        <v>327.27273000000002</v>
+      </c>
+      <c r="E615" s="1">
+        <f t="shared" si="93"/>
+        <v>418.90909440000007</v>
+      </c>
+      <c r="G615" s="3">
+        <v>3</v>
+      </c>
+      <c r="H615" s="3">
+        <v>315.78946999999999</v>
+      </c>
+      <c r="I615" s="1">
+        <f t="shared" si="94"/>
+        <v>404.21052159999999</v>
+      </c>
+    </row>
+    <row r="616" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C616" s="3">
+        <v>4</v>
+      </c>
+      <c r="D616" s="3">
+        <v>381.81817999999998</v>
+      </c>
+      <c r="E616" s="1">
+        <f t="shared" si="93"/>
+        <v>488.72727040000001</v>
+      </c>
+      <c r="G616" s="3">
+        <v>4</v>
+      </c>
+      <c r="H616" s="3">
+        <v>378.94736999999998</v>
+      </c>
+      <c r="I616" s="1">
+        <f t="shared" si="94"/>
+        <v>485.05263359999998</v>
+      </c>
+    </row>
+    <row r="617" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C617" s="3">
+        <v>5</v>
+      </c>
+      <c r="D617" s="3">
+        <v>490.90908999999999</v>
+      </c>
+      <c r="E617" s="1">
+        <f t="shared" si="93"/>
+        <v>628.36363519999998</v>
+      </c>
+      <c r="G617" s="3">
+        <v>5</v>
+      </c>
+      <c r="H617" s="3">
+        <v>505.26316000000003</v>
+      </c>
+      <c r="I617" s="1">
+        <f t="shared" si="94"/>
+        <v>646.73684480000009</v>
+      </c>
+    </row>
+    <row r="618" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C618" s="3">
+        <v>6</v>
+      </c>
+      <c r="D618" s="3">
+        <v>600</v>
+      </c>
+      <c r="E618" s="1">
+        <f t="shared" si="93"/>
+        <v>768</v>
+      </c>
+      <c r="G618" s="3">
+        <v>6</v>
+      </c>
+      <c r="H618" s="3">
+        <v>568.42105000000004</v>
+      </c>
+      <c r="I618" s="1">
+        <f t="shared" si="94"/>
+        <v>727.57894400000009</v>
+      </c>
+    </row>
+    <row r="619" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C619" s="3">
+        <v>7</v>
+      </c>
+      <c r="D619" s="3">
+        <v>654.54544999999996</v>
+      </c>
+      <c r="E619" s="1">
+        <f t="shared" si="93"/>
+        <v>837.81817599999999</v>
+      </c>
+      <c r="G619" s="3">
+        <v>7</v>
+      </c>
+      <c r="H619" s="3">
+        <v>694.73684000000003</v>
+      </c>
+      <c r="I619" s="1">
+        <f t="shared" si="94"/>
+        <v>889.26315520000003</v>
+      </c>
+    </row>
+    <row r="620" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C620" s="3">
+        <v>8</v>
+      </c>
+      <c r="D620" s="3">
+        <v>763.63635999999997</v>
+      </c>
+      <c r="E620" s="1">
+        <f t="shared" si="93"/>
+        <v>977.45454080000002</v>
+      </c>
+      <c r="G620" s="3">
+        <v>8</v>
+      </c>
+      <c r="H620" s="3">
+        <v>757.89473999999996</v>
+      </c>
+      <c r="I620" s="1">
+        <f t="shared" si="94"/>
+        <v>970.10526719999996</v>
+      </c>
+    </row>
+    <row r="621" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C621" s="3">
+        <v>9</v>
+      </c>
+      <c r="D621">
+        <v>872.72726999999998</v>
+      </c>
+      <c r="E621" s="1">
+        <f t="shared" si="93"/>
+        <v>1117.0909056</v>
+      </c>
+      <c r="G621" s="3">
+        <v>9</v>
+      </c>
+      <c r="H621">
+        <v>884.21052999999995</v>
+      </c>
+      <c r="I621" s="1">
+        <f t="shared" si="94"/>
+        <v>1131.7894784</v>
+      </c>
+    </row>
+    <row r="622" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C622" s="3">
+        <v>10</v>
+      </c>
+      <c r="D622" s="3">
+        <v>927.27273000000002</v>
+      </c>
+      <c r="E622" s="1">
+        <f t="shared" si="93"/>
+        <v>1186.9090944</v>
+      </c>
+      <c r="G622" s="3">
+        <v>10</v>
+      </c>
+      <c r="H622" s="3">
+        <v>947.36842000000001</v>
+      </c>
+      <c r="I622" s="1">
+        <f t="shared" si="94"/>
+        <v>1212.6315776000001</v>
+      </c>
+    </row>
+    <row r="623" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C623" s="3">
+        <v>11</v>
+      </c>
+      <c r="D623">
+        <v>1036.36364</v>
+      </c>
+      <c r="E623" s="1">
+        <f t="shared" si="93"/>
+        <v>1326.5454592000001</v>
+      </c>
+      <c r="G623" s="3">
+        <v>11</v>
+      </c>
+      <c r="H623">
+        <v>1073.6842099999999</v>
+      </c>
+      <c r="I623" s="1">
+        <f t="shared" si="94"/>
+        <v>1374.3157887999998</v>
+      </c>
+    </row>
+    <row r="624" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C624" s="3">
+        <v>12</v>
+      </c>
+      <c r="D624" s="3">
+        <v>1145.4545499999999</v>
+      </c>
+      <c r="E624" s="1">
+        <f t="shared" si="93"/>
+        <v>1466.1818239999998</v>
+      </c>
+      <c r="G624" s="3">
+        <v>12</v>
+      </c>
+      <c r="H624" s="3">
+        <v>1136.84211</v>
+      </c>
+      <c r="I624" s="1">
+        <f t="shared" si="94"/>
+        <v>1455.1579008000001</v>
+      </c>
+    </row>
+    <row r="625" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C625" s="3">
+        <v>13</v>
+      </c>
+      <c r="D625">
+        <v>1200</v>
+      </c>
+      <c r="E625" s="1">
+        <f t="shared" si="93"/>
+        <v>1536</v>
+      </c>
+      <c r="G625" s="3">
+        <v>13</v>
+      </c>
+      <c r="H625">
+        <v>1200</v>
+      </c>
+      <c r="I625" s="1">
+        <f t="shared" si="94"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="629" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C629" t="s">
+        <v>100</v>
+      </c>
+      <c r="E629" t="s">
+        <v>103</v>
+      </c>
+      <c r="G629" t="s">
+        <v>101</v>
+      </c>
+      <c r="N629" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="630" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C630" s="3"/>
+      <c r="D630" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E630" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G630" s="3"/>
+      <c r="H630" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I630" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="631" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C631" s="3">
+        <v>0</v>
+      </c>
+      <c r="D631" s="3">
+        <v>0</v>
+      </c>
+      <c r="E631" s="1">
+        <f>(D631/$D$647)*1536</f>
+        <v>0</v>
+      </c>
+      <c r="G631" s="3">
+        <v>0</v>
+      </c>
+      <c r="H631" s="3">
+        <v>0</v>
+      </c>
+      <c r="I631" s="1">
+        <f>(H631/$H$647)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C632" s="3">
+        <v>1</v>
+      </c>
+      <c r="D632" s="3">
+        <v>148.96552</v>
+      </c>
+      <c r="E632" s="1">
+        <f t="shared" ref="E632:E647" si="95">(D632/$D$647)*1536</f>
+        <v>190.67586559999998</v>
+      </c>
+      <c r="G632" s="3">
+        <v>1</v>
+      </c>
+      <c r="H632" s="3">
+        <v>77.697839999999999</v>
+      </c>
+      <c r="I632" s="1">
+        <f t="shared" ref="I632:I647" si="96">(H632/$H$647)*1536</f>
+        <v>99.453235200000009</v>
+      </c>
+    </row>
+    <row r="633" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C633" s="3">
+        <v>2</v>
+      </c>
+      <c r="D633" s="3">
+        <v>206.89654999999999</v>
+      </c>
+      <c r="E633" s="1">
+        <f t="shared" si="95"/>
+        <v>264.827584</v>
+      </c>
+      <c r="G633" s="3">
+        <v>2</v>
+      </c>
+      <c r="H633" s="3">
+        <v>155.39568</v>
+      </c>
+      <c r="I633" s="1">
+        <f t="shared" si="96"/>
+        <v>198.90647040000002</v>
+      </c>
+    </row>
+    <row r="634" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C634" s="3">
+        <v>3</v>
+      </c>
+      <c r="D634" s="3">
+        <v>264.82758999999999</v>
+      </c>
+      <c r="E634" s="1">
+        <f t="shared" si="95"/>
+        <v>338.97931519999997</v>
+      </c>
+      <c r="G634" s="3">
+        <v>3</v>
+      </c>
+      <c r="H634" s="3">
+        <v>233.09352999999999</v>
+      </c>
+      <c r="I634" s="1">
+        <f t="shared" si="96"/>
+        <v>298.35971839999996</v>
+      </c>
+    </row>
+    <row r="635" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C635" s="3">
+        <v>4</v>
+      </c>
+      <c r="D635" s="3">
+        <v>322.75862000000001</v>
+      </c>
+      <c r="E635" s="1">
+        <f t="shared" si="95"/>
+        <v>413.13103360000002</v>
+      </c>
+      <c r="G635" s="3">
+        <v>4</v>
+      </c>
+      <c r="H635" s="3">
+        <v>310.79136999999997</v>
+      </c>
+      <c r="I635" s="1">
+        <f t="shared" si="96"/>
+        <v>397.81295360000001</v>
+      </c>
+    </row>
+    <row r="636" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C636" s="3">
+        <v>5</v>
+      </c>
+      <c r="D636" s="3">
+        <v>380.68966</v>
+      </c>
+      <c r="E636" s="1">
+        <f t="shared" si="95"/>
+        <v>487.2827648</v>
+      </c>
+      <c r="G636" s="3">
+        <v>5</v>
+      </c>
+      <c r="H636" s="3">
+        <v>388.48921000000001</v>
+      </c>
+      <c r="I636" s="1">
+        <f t="shared" si="96"/>
+        <v>497.26618880000001</v>
+      </c>
+    </row>
+    <row r="637" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C637" s="3">
+        <v>6</v>
+      </c>
+      <c r="D637" s="3">
+        <v>438.62069000000002</v>
+      </c>
+      <c r="E637" s="1">
+        <f t="shared" si="95"/>
+        <v>561.43448320000005</v>
+      </c>
+      <c r="G637" s="3">
+        <v>6</v>
+      </c>
+      <c r="H637" s="3">
+        <v>466.18705</v>
+      </c>
+      <c r="I637" s="1">
+        <f t="shared" si="96"/>
+        <v>596.719424</v>
+      </c>
+    </row>
+    <row r="638" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C638" s="3">
+        <v>7</v>
+      </c>
+      <c r="D638" s="3">
+        <v>587.58621000000005</v>
+      </c>
+      <c r="E638" s="1">
+        <f t="shared" si="95"/>
+        <v>752.11034880000011</v>
+      </c>
+      <c r="G638" s="3">
+        <v>7</v>
+      </c>
+      <c r="H638" s="3">
+        <v>543.88489000000004</v>
+      </c>
+      <c r="I638" s="1">
+        <f t="shared" si="96"/>
+        <v>696.1726592</v>
+      </c>
+    </row>
+    <row r="639" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C639" s="3">
+        <v>8</v>
+      </c>
+      <c r="D639" s="3">
+        <v>645.51724000000002</v>
+      </c>
+      <c r="E639" s="1">
+        <f t="shared" si="95"/>
+        <v>826.26206720000005</v>
+      </c>
+      <c r="G639" s="3">
+        <v>8</v>
+      </c>
+      <c r="H639" s="3">
+        <v>621.58272999999997</v>
+      </c>
+      <c r="I639" s="1">
+        <f t="shared" si="96"/>
+        <v>795.62589439999988</v>
+      </c>
+    </row>
+    <row r="640" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C640" s="3">
+        <v>9</v>
+      </c>
+      <c r="D640">
+        <v>703.44827999999995</v>
+      </c>
+      <c r="E640" s="1">
+        <f t="shared" si="95"/>
+        <v>900.41379839999991</v>
+      </c>
+      <c r="G640" s="3">
+        <v>9</v>
+      </c>
+      <c r="H640">
+        <v>699.28057999999999</v>
+      </c>
+      <c r="I640" s="1">
+        <f t="shared" si="96"/>
+        <v>895.07914240000002</v>
+      </c>
+    </row>
+    <row r="641" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C641" s="3">
+        <v>10</v>
+      </c>
+      <c r="D641" s="3">
+        <v>761.37931000000003</v>
+      </c>
+      <c r="E641" s="1">
+        <f t="shared" si="95"/>
+        <v>974.56551680000007</v>
+      </c>
+      <c r="G641" s="3">
+        <v>10</v>
+      </c>
+      <c r="H641" s="3">
+        <v>776.97842000000003</v>
+      </c>
+      <c r="I641" s="1">
+        <f t="shared" si="96"/>
+        <v>994.53237760000002</v>
+      </c>
+    </row>
+    <row r="642" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C642" s="3">
+        <v>11</v>
+      </c>
+      <c r="D642">
+        <v>819.31034</v>
+      </c>
+      <c r="E642" s="1">
+        <f t="shared" si="95"/>
+        <v>1048.7172352</v>
+      </c>
+      <c r="G642" s="3">
+        <v>11</v>
+      </c>
+      <c r="H642">
+        <v>854.67625999999996</v>
+      </c>
+      <c r="I642" s="1">
+        <f t="shared" si="96"/>
+        <v>1093.9856127999999</v>
+      </c>
+    </row>
+    <row r="643" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C643" s="3">
+        <v>12</v>
+      </c>
+      <c r="D643" s="3">
+        <v>968.27585999999997</v>
+      </c>
+      <c r="E643" s="1">
+        <f t="shared" si="95"/>
+        <v>1239.3931008</v>
+      </c>
+      <c r="G643" s="3">
+        <v>12</v>
+      </c>
+      <c r="H643" s="3">
+        <v>932.3741</v>
+      </c>
+      <c r="I643" s="1">
+        <f t="shared" si="96"/>
+        <v>1193.438848</v>
+      </c>
+    </row>
+    <row r="644" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C644" s="3">
+        <v>13</v>
+      </c>
+      <c r="D644">
+        <v>1026.2068999999999</v>
+      </c>
+      <c r="E644" s="1">
+        <f t="shared" si="95"/>
+        <v>1313.5448319999998</v>
+      </c>
+      <c r="G644" s="3">
+        <v>13</v>
+      </c>
+      <c r="H644">
+        <v>1010.07194</v>
+      </c>
+      <c r="I644" s="1">
+        <f t="shared" si="96"/>
+        <v>1292.8920832000001</v>
+      </c>
+    </row>
+    <row r="645" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C645" s="3">
+        <v>14</v>
+      </c>
+      <c r="D645">
+        <v>1084.1379300000001</v>
+      </c>
+      <c r="E645" s="1">
+        <f t="shared" si="95"/>
+        <v>1387.6965504000002</v>
+      </c>
+      <c r="G645" s="3">
+        <v>14</v>
+      </c>
+      <c r="H645">
+        <v>1087.7697800000001</v>
+      </c>
+      <c r="I645" s="1">
+        <f t="shared" si="96"/>
+        <v>1392.3453184</v>
+      </c>
+    </row>
+    <row r="646" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C646" s="3">
+        <v>15</v>
+      </c>
+      <c r="D646">
+        <v>1142.06897</v>
+      </c>
+      <c r="E646" s="1">
+        <f t="shared" si="95"/>
+        <v>1461.8482816000001</v>
+      </c>
+      <c r="G646" s="3">
+        <v>15</v>
+      </c>
+      <c r="H646">
+        <v>1165.4676300000001</v>
+      </c>
+      <c r="I646" s="1">
+        <f t="shared" si="96"/>
+        <v>1491.7985664000003</v>
+      </c>
+    </row>
+    <row r="647" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C647" s="3">
+        <v>16</v>
+      </c>
+      <c r="D647">
+        <v>1200</v>
+      </c>
+      <c r="E647" s="1">
+        <f t="shared" si="95"/>
+        <v>1536</v>
+      </c>
+      <c r="G647" s="3">
+        <v>16</v>
+      </c>
+      <c r="H647">
+        <v>1200</v>
+      </c>
+      <c r="I647" s="1">
+        <f t="shared" si="96"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="651" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C651" t="s">
+        <v>102</v>
+      </c>
+      <c r="F651" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="652" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C652" s="3"/>
+      <c r="D652" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E652" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="653" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C653" s="3">
+        <v>0</v>
+      </c>
+      <c r="D653" s="3">
+        <v>0</v>
+      </c>
+      <c r="E653" s="1">
+        <f>(D653/$D$669)*1536</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C654" s="3">
+        <v>1</v>
+      </c>
+      <c r="D654" s="3">
+        <v>77.419349999999994</v>
+      </c>
+      <c r="E654" s="1">
+        <f t="shared" ref="E654:E669" si="97">(D654/$D$669)*1536</f>
+        <v>99.096767999999997</v>
+      </c>
+    </row>
+    <row r="655" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C655" s="3">
+        <v>2</v>
+      </c>
+      <c r="D655" s="3">
+        <v>154.83870999999999</v>
+      </c>
+      <c r="E655" s="1">
+        <f t="shared" si="97"/>
+        <v>198.19354879999997</v>
+      </c>
+    </row>
+    <row r="656" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C656" s="3">
+        <v>3</v>
+      </c>
+      <c r="D656" s="3">
+        <v>232.25806</v>
+      </c>
+      <c r="E656" s="1">
+        <f t="shared" si="97"/>
+        <v>297.29031679999997</v>
+      </c>
+    </row>
+    <row r="657" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C657" s="3">
+        <v>4</v>
+      </c>
+      <c r="D657" s="3">
+        <v>309.67741999999998</v>
+      </c>
+      <c r="E657" s="1">
+        <f t="shared" si="97"/>
+        <v>396.38709759999995</v>
+      </c>
+    </row>
+    <row r="658" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C658" s="3">
+        <v>5</v>
+      </c>
+      <c r="D658" s="3">
+        <v>387.09676999999999</v>
+      </c>
+      <c r="E658" s="1">
+        <f t="shared" si="97"/>
+        <v>495.4838656</v>
+      </c>
+    </row>
+    <row r="659" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C659" s="3">
+        <v>6</v>
+      </c>
+      <c r="D659" s="3">
+        <v>464.51612999999998</v>
+      </c>
+      <c r="E659" s="1">
+        <f t="shared" si="97"/>
+        <v>594.58064639999998</v>
+      </c>
+    </row>
+    <row r="660" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C660" s="3">
+        <v>7</v>
+      </c>
+      <c r="D660" s="3">
+        <v>541.93547999999998</v>
+      </c>
+      <c r="E660" s="1">
+        <f t="shared" si="97"/>
+        <v>693.67741439999998</v>
+      </c>
+    </row>
+    <row r="661" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C661" s="3">
+        <v>8</v>
+      </c>
+      <c r="D661" s="3">
+        <v>619.35483999999997</v>
+      </c>
+      <c r="E661" s="1">
+        <f t="shared" si="97"/>
+        <v>792.77419519999989</v>
+      </c>
+    </row>
+    <row r="662" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C662" s="3">
+        <v>9</v>
+      </c>
+      <c r="D662">
+        <v>696.77418999999998</v>
+      </c>
+      <c r="E662" s="1">
+        <f t="shared" si="97"/>
+        <v>891.87096320000001</v>
+      </c>
+    </row>
+    <row r="663" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C663" s="3">
+        <v>10</v>
+      </c>
+      <c r="D663" s="3">
+        <v>774.19354999999996</v>
+      </c>
+      <c r="E663" s="1">
+        <f t="shared" si="97"/>
+        <v>990.96774399999981</v>
+      </c>
+    </row>
+    <row r="664" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C664" s="3">
+        <v>11</v>
+      </c>
+      <c r="D664">
+        <v>851.61289999999997</v>
+      </c>
+      <c r="E664" s="1">
+        <f t="shared" si="97"/>
+        <v>1090.0645119999999</v>
+      </c>
+    </row>
+    <row r="665" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C665" s="3">
+        <v>12</v>
+      </c>
+      <c r="D665" s="3">
+        <v>929.03225999999995</v>
+      </c>
+      <c r="E665" s="1">
+        <f t="shared" si="97"/>
+        <v>1189.1612928</v>
+      </c>
+    </row>
+    <row r="666" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C666" s="3">
+        <v>13</v>
+      </c>
+      <c r="D666">
+        <v>967.74194</v>
+      </c>
+      <c r="E666" s="1">
+        <f t="shared" si="97"/>
+        <v>1238.7096832</v>
+      </c>
+    </row>
+    <row r="667" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C667" s="3">
+        <v>14</v>
+      </c>
+      <c r="D667">
+        <v>1045.16129</v>
+      </c>
+      <c r="E667" s="1">
+        <f t="shared" si="97"/>
+        <v>1337.8064512000001</v>
+      </c>
+    </row>
+    <row r="668" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C668" s="3">
+        <v>15</v>
+      </c>
+      <c r="D668">
+        <v>1122.5806500000001</v>
+      </c>
+      <c r="E668" s="1">
+        <f t="shared" si="97"/>
+        <v>1436.9032320000001</v>
+      </c>
+    </row>
+    <row r="669" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C669" s="3">
+        <v>16</v>
+      </c>
+      <c r="D669">
+        <v>1200</v>
+      </c>
+      <c r="E669" s="1">
+        <f t="shared" si="97"/>
         <v>1536</v>
       </c>
     </row>

</xml_diff>